<commit_message>
log results to text file
</commit_message>
<xml_diff>
--- a/training_data.xlsx
+++ b/training_data.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Setosa" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Versicolor" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Virginica" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test Data &amp; Results" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,16 +465,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -484,16 +484,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.9</v>
+        <v>5.4</v>
       </c>
       <c r="B3" t="n">
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="C3" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -503,16 +503,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="B4" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="C4" t="n">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -522,13 +522,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="C5" t="n">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="D5" t="n">
         <v>0.2</v>
@@ -541,16 +541,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5.1</v>
+        <v>5.2</v>
       </c>
       <c r="B6" t="n">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -560,10 +560,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.1</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="C7" t="n">
         <v>1.4</v>
@@ -579,16 +579,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5.1</v>
+        <v>4.7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="C8" t="n">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -598,16 +598,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4.4</v>
+        <v>4.8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -617,13 +617,13 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="B10" t="n">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="C10" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D10" t="n">
         <v>0.2</v>
@@ -636,16 +636,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="B11" t="n">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="C11" t="n">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -655,13 +655,13 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="B12" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="C12" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="D12" t="n">
         <v>0.2</v>
@@ -674,16 +674,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5.4</v>
+        <v>4.6</v>
       </c>
       <c r="B13" t="n">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
       <c r="C13" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -693,16 +693,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4.8</v>
+        <v>5.1</v>
       </c>
       <c r="B14" t="n">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="C14" t="n">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -712,16 +712,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>5.1</v>
       </c>
       <c r="B15" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="C15" t="n">
         <v>1.5</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -731,16 +731,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="B16" t="n">
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -750,16 +750,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="B17" t="n">
-        <v>3.7</v>
+        <v>4.1</v>
       </c>
       <c r="C17" t="n">
         <v>1.5</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -769,16 +769,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4.6</v>
+        <v>4.9</v>
       </c>
       <c r="B18" t="n">
         <v>3.6</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -788,13 +788,13 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>5.1</v>
+        <v>4.9</v>
       </c>
       <c r="B19" t="n">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
       <c r="C19" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D19" t="n">
         <v>0.2</v>
@@ -807,13 +807,13 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="B20" t="n">
-        <v>2.3</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="D20" t="n">
         <v>0.3</v>
@@ -826,16 +826,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>5</v>
+        <v>5.7</v>
       </c>
       <c r="B21" t="n">
-        <v>3.5</v>
+        <v>4.4</v>
       </c>
       <c r="C21" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -845,13 +845,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>5</v>
+        <v>5.1</v>
       </c>
       <c r="B22" t="n">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="C22" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="D22" t="n">
         <v>0.2</v>
@@ -864,13 +864,13 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="B23" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C23" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="D23" t="n">
         <v>0.2</v>
@@ -883,16 +883,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>5.1</v>
+        <v>4.8</v>
       </c>
       <c r="B24" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C24" t="n">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -902,13 +902,13 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4.9</v>
+        <v>5.1</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="C25" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D25" t="n">
         <v>0.2</v>
@@ -924,10 +924,10 @@
         <v>4.6</v>
       </c>
       <c r="B26" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C26" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D26" t="n">
         <v>0.2</v>
@@ -940,10 +940,10 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>5.2</v>
+        <v>4.9</v>
       </c>
       <c r="B27" t="n">
-        <v>4.1</v>
+        <v>3.1</v>
       </c>
       <c r="C27" t="n">
         <v>1.5</v>
@@ -959,16 +959,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="B28" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="C28" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="D28" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -978,13 +978,13 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>4.9</v>
+        <v>4.3</v>
       </c>
       <c r="B29" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="D29" t="n">
         <v>0.1</v>
@@ -997,16 +997,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="B30" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="C30" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1016,16 +1016,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5.4</v>
+        <v>5.3</v>
       </c>
       <c r="B31" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="C31" t="n">
         <v>1.5</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1038,13 +1038,13 @@
         <v>4.8</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C32" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1054,16 +1054,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>4.9</v>
+        <v>4.5</v>
       </c>
       <c r="B33" t="n">
-        <v>3.1</v>
+        <v>2.3</v>
       </c>
       <c r="C33" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="B34" t="n">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
       <c r="C34" t="n">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="D34" t="n">
         <v>0.4</v>
@@ -1111,16 +1111,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>5.7</v>
+        <v>5.1</v>
       </c>
       <c r="B36" t="n">
-        <v>4.4</v>
+        <v>3.3</v>
       </c>
       <c r="C36" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="D36" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1130,16 +1130,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>4.6</v>
+        <v>4.9</v>
       </c>
       <c r="B37" t="n">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C37" t="n">
         <v>1.4</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1149,13 +1149,13 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>4.4</v>
+        <v>5</v>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="C38" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D38" t="n">
         <v>0.2</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>5.1</v>
+        <v>5.4</v>
       </c>
       <c r="B39" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="C39" t="n">
         <v>1.5</v>
@@ -1196,7 +1196,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,16 +1233,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C2" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1252,16 +1252,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="B3" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="C3" t="n">
-        <v>4.7</v>
+        <v>3.9</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1271,16 +1271,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="B4" t="n">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="C4" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="D4" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1290,16 +1290,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.5</v>
+        <v>5.2</v>
       </c>
       <c r="B5" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="D5" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1309,16 +1309,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="D6" t="n">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1328,16 +1328,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2.3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1347,16 +1347,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6.6</v>
+        <v>4.9</v>
       </c>
       <c r="B8" t="n">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="C8" t="n">
-        <v>4.6</v>
+        <v>3.3</v>
       </c>
       <c r="D8" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1366,13 +1366,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="B9" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>4.9</v>
+        <v>4.5</v>
       </c>
       <c r="D9" t="n">
         <v>1.5</v>
@@ -1385,16 +1385,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>6.1</v>
       </c>
       <c r="B10" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="C10" t="n">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1404,16 +1404,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5.8</v>
+        <v>6.4</v>
       </c>
       <c r="B11" t="n">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="D11" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1423,16 +1423,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="C12" t="n">
-        <v>3.5</v>
+        <v>4.3</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1442,16 +1442,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5.6</v>
+        <v>6.3</v>
       </c>
       <c r="B13" t="n">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="C13" t="n">
-        <v>4.2</v>
+        <v>4.9</v>
       </c>
       <c r="D13" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1461,16 +1461,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="B14" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="C14" t="n">
-        <v>4.1</v>
+        <v>3.6</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1480,16 +1480,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="C15" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="D15" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1499,16 +1499,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C16" t="n">
         <v>5.1</v>
       </c>
-      <c r="B16" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="C16" t="n">
-        <v>3</v>
-      </c>
       <c r="D16" t="n">
-        <v>1.1</v>
+        <v>1.6</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1518,16 +1518,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>4.9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="C17" t="n">
-        <v>3.3</v>
+        <v>4.5</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1537,16 +1537,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="B18" t="n">
-        <v>2.2</v>
+        <v>2.7</v>
       </c>
       <c r="C18" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="D18" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>5.7</v>
+        <v>5.9</v>
       </c>
       <c r="B19" t="n">
         <v>3</v>
@@ -1565,7 +1565,7 @@
         <v>4.2</v>
       </c>
       <c r="D19" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1575,16 +1575,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="B20" t="n">
-        <v>2.2</v>
+        <v>3.1</v>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>4.9</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1594,16 +1594,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="B21" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="C21" t="n">
-        <v>4.4</v>
+        <v>4.7</v>
       </c>
       <c r="D21" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1613,13 +1613,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="B22" t="n">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="C22" t="n">
-        <v>4.7</v>
+        <v>3.9</v>
       </c>
       <c r="D22" t="n">
         <v>1.2</v>
@@ -1632,16 +1632,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5.7</v>
+        <v>6.3</v>
       </c>
       <c r="B23" t="n">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="C23" t="n">
-        <v>3.5</v>
+        <v>4.4</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1651,16 +1651,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="B24" t="n">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D24" t="n">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1673,10 +1673,10 @@
         <v>5.7</v>
       </c>
       <c r="B25" t="n">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="C25" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="D25" t="n">
         <v>1.3</v>
@@ -1689,16 +1689,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>6.8</v>
+        <v>5.5</v>
       </c>
       <c r="B26" t="n">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="C26" t="n">
-        <v>4.8</v>
+        <v>3.7</v>
       </c>
       <c r="D26" t="n">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1708,16 +1708,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="B27" t="n">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C27" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D27" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1727,16 +1727,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>7</v>
+        <v>5.6</v>
       </c>
       <c r="B28" t="n">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>4.7</v>
+        <v>4.1</v>
       </c>
       <c r="D28" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1746,13 +1746,13 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="B29" t="n">
-        <v>2.9</v>
+        <v>2.3</v>
       </c>
       <c r="C29" t="n">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="D29" t="n">
         <v>1.3</v>
@@ -1765,16 +1765,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>5.6</v>
+        <v>6.7</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C30" t="n">
-        <v>4.5</v>
+        <v>4.4</v>
       </c>
       <c r="D30" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1790,10 +1790,10 @@
         <v>2.4</v>
       </c>
       <c r="C31" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1803,16 +1803,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>6</v>
+        <v>5.9</v>
       </c>
       <c r="B32" t="n">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="C32" t="n">
-        <v>5.1</v>
+        <v>4.8</v>
       </c>
       <c r="D32" t="n">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1822,56 +1822,18 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>5.2</v>
+        <v>5.8</v>
       </c>
       <c r="B33" t="n">
         <v>2.7</v>
       </c>
       <c r="C33" t="n">
-        <v>3.9</v>
+        <v>4.1</v>
       </c>
       <c r="D33" t="n">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
-        <is>
-          <t>Iris-versicolor</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>6</v>
-      </c>
-      <c r="B34" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="C34" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D34" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Iris-versicolor</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="B35" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D35" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E35" t="inlineStr">
         <is>
           <t>Iris-versicolor</t>
         </is>
@@ -1888,7 +1850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1925,16 +1887,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="C2" t="n">
-        <v>5.1</v>
+        <v>5.6</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1944,16 +1906,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
       <c r="B3" t="n">
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1963,16 +1925,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="B4" t="n">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>5.1</v>
       </c>
       <c r="D4" t="n">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1982,13 +1944,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="B5" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="C5" t="n">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="D5" t="n">
         <v>1.8</v>
@@ -2001,16 +1963,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7.4</v>
+        <v>6.3</v>
       </c>
       <c r="B6" t="n">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="C6" t="n">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="D6" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -2020,16 +1982,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C7" t="n">
-        <v>4.8</v>
+        <v>5.6</v>
       </c>
       <c r="D7" t="n">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2039,16 +2001,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.7</v>
+        <v>4.9</v>
       </c>
       <c r="B8" t="n">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="C8" t="n">
-        <v>6.9</v>
+        <v>4.5</v>
       </c>
       <c r="D8" t="n">
-        <v>2.3</v>
+        <v>1.7</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2058,16 +2020,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C9" t="n">
-        <v>5.5</v>
+        <v>4.9</v>
       </c>
       <c r="D9" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2096,16 +2058,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="B11" t="n">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="C11" t="n">
-        <v>5.1</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2115,16 +2077,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7.7</v>
+        <v>7.4</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C12" t="n">
         <v>6.1</v>
       </c>
       <c r="D12" t="n">
-        <v>2.3</v>
+        <v>1.9</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2134,16 +2096,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5.6</v>
+        <v>7.1</v>
       </c>
       <c r="B13" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>4.9</v>
+        <v>5.9</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2153,13 +2115,13 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6.8</v>
+        <v>7.7</v>
       </c>
       <c r="B14" t="n">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="C14" t="n">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="D14" t="n">
         <v>2.3</v>
@@ -2172,16 +2134,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7.7</v>
+        <v>6.8</v>
       </c>
       <c r="B15" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="C15" t="n">
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>2.3</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2191,13 +2153,13 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="B16" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>5.1</v>
+        <v>5.2</v>
       </c>
       <c r="D16" t="n">
         <v>2.3</v>
@@ -2210,16 +2172,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="B17" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="D17" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2229,16 +2191,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="B18" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="D18" t="n">
-        <v>2.2</v>
+        <v>1.8</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2248,16 +2210,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
       <c r="B19" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="C19" t="n">
-        <v>5.7</v>
+        <v>5.1</v>
       </c>
       <c r="D19" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2267,13 +2229,13 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>6.2</v>
+        <v>6.9</v>
       </c>
       <c r="B20" t="n">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="C20" t="n">
-        <v>5.4</v>
+        <v>5.1</v>
       </c>
       <c r="D20" t="n">
         <v>2.3</v>
@@ -2286,16 +2248,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6.4</v>
+        <v>7.7</v>
       </c>
       <c r="B21" t="n">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="C21" t="n">
-        <v>5.3</v>
+        <v>6.7</v>
       </c>
       <c r="D21" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2311,10 +2273,10 @@
         <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
       <c r="D22" t="n">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2324,16 +2286,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="B23" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="C23" t="n">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="D23" t="n">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2343,16 +2305,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>7.2</v>
+        <v>6.9</v>
       </c>
       <c r="B24" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="C24" t="n">
-        <v>6.1</v>
+        <v>5.7</v>
       </c>
       <c r="D24" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -2362,16 +2324,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>6.7</v>
+        <v>5.6</v>
       </c>
       <c r="B25" t="n">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="C25" t="n">
-        <v>5.6</v>
+        <v>4.9</v>
       </c>
       <c r="D25" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -2381,16 +2343,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="B26" t="n">
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="C26" t="n">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="D26" t="n">
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -2400,13 +2362,13 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>6.3</v>
+        <v>7.2</v>
       </c>
       <c r="B27" t="n">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="C27" t="n">
-        <v>4.9</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
         <v>1.8</v>
@@ -2419,16 +2381,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>6.1</v>
+        <v>7.9</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="C28" t="n">
-        <v>4.9</v>
+        <v>6.4</v>
       </c>
       <c r="D28" t="n">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -2438,16 +2400,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="B29" t="n">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="C29" t="n">
-        <v>5.1</v>
+        <v>5</v>
       </c>
       <c r="D29" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2457,16 +2419,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>7.1</v>
+        <v>6.7</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="C30" t="n">
-        <v>5.9</v>
+        <v>5.7</v>
       </c>
       <c r="D30" t="n">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2476,16 +2438,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5.9</v>
+        <v>6.4</v>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="C31" t="n">
-        <v>5.1</v>
+        <v>5.3</v>
       </c>
       <c r="D31" t="n">
-        <v>1.8</v>
+        <v>2.3</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2495,16 +2457,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>6</v>
+        <v>5.8</v>
       </c>
       <c r="B32" t="n">
-        <v>2.2</v>
+        <v>2.7</v>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>5.1</v>
       </c>
       <c r="D32" t="n">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2514,16 +2476,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C33" t="n">
-        <v>5.2</v>
+        <v>5.3</v>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -2533,18 +2495,56 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7.9</v>
+        <v>7.2</v>
       </c>
       <c r="B34" t="n">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>6.4</v>
+        <v>5.8</v>
       </c>
       <c r="D34" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Iris-virginica</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C35" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="D35" t="n">
         <v>2</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Iris-virginica</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>Iris-virginica</t>
         </is>
@@ -2597,29 +2597,29 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Guesses</t>
+          <t>Mean only</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Guesses2</t>
+          <t>Mean/SD</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Guesses3</t>
+          <t>Median</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4.7</v>
+        <v>5.1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="D2" t="n">
         <v>0.2</v>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D3" t="n">
         <v>0.2</v>
@@ -2681,16 +2681,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="C4" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -2715,16 +2715,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.1</v>
+        <v>4.8</v>
       </c>
       <c r="B5" t="n">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -2749,13 +2749,13 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="B6" t="n">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="D6" t="n">
         <v>0.2</v>
@@ -2783,16 +2783,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.1</v>
+        <v>5.4</v>
       </c>
       <c r="B7" t="n">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="C7" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2817,16 +2817,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4.8</v>
+        <v>5.1</v>
       </c>
       <c r="B8" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="C8" t="n">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2851,13 +2851,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="C9" t="n">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0.2</v>
@@ -2885,13 +2885,13 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="B10" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D10" t="n">
         <v>0.2</v>
@@ -2919,16 +2919,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4.7</v>
+        <v>5.4</v>
       </c>
       <c r="B11" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="C11" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="B12" t="n">
         <v>3.5</v>
@@ -2962,7 +2962,7 @@
         <v>1.3</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2987,16 +2987,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4.6</v>
+        <v>5.1</v>
       </c>
       <c r="B13" t="n">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="C13" t="n">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -3021,16 +3021,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6.9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C14" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="D14" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="B15" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="C15" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="D15" t="n">
         <v>1.5</v>
@@ -3089,16 +3089,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="B16" t="n">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="C16" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="D16" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3112,27 +3112,27 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5.9</v>
+        <v>5.7</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C17" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="D17" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -3157,16 +3157,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>5.6</v>
+        <v>6.3</v>
       </c>
       <c r="B18" t="n">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="C18" t="n">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
       <c r="D18" t="n">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3180,27 +3180,27 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>5.6</v>
+        <v>6</v>
       </c>
       <c r="B19" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="C19" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3225,16 +3225,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>5.9</v>
+        <v>5.6</v>
       </c>
       <c r="B20" t="n">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="D20" t="n">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -3259,16 +3259,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="B21" t="n">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="C21" t="n">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="D21" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3327,16 +3327,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="B23" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="C23" t="n">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="D23" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -3361,16 +3361,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>5.8</v>
+        <v>6.7</v>
       </c>
       <c r="B24" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>3.9</v>
+        <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3379,32 +3379,32 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="B25" t="n">
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="C25" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D25" t="n">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3463,16 +3463,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C27" t="n">
-        <v>4.1</v>
+        <v>4.4</v>
       </c>
       <c r="D27" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -3497,16 +3497,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="B28" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>4.3</v>
+        <v>4.6</v>
       </c>
       <c r="D28" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -3531,16 +3531,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="B29" t="n">
-        <v>2.8</v>
+        <v>2.3</v>
       </c>
       <c r="C29" t="n">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="D29" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -3565,84 +3565,84 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>6.5</v>
+        <v>5.7</v>
       </c>
       <c r="B30" t="n">
         <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>5.8</v>
+        <v>4.2</v>
       </c>
       <c r="D30" t="n">
-        <v>2.2</v>
+        <v>1.2</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>7.6</v>
+        <v>5.1</v>
       </c>
       <c r="B31" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C31" t="n">
         <v>3</v>
       </c>
-      <c r="C31" t="n">
-        <v>6.6</v>
-      </c>
       <c r="D31" t="n">
-        <v>2.1</v>
+        <v>1.1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>4.9</v>
+        <v>7.3</v>
       </c>
       <c r="B32" t="n">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="C32" t="n">
-        <v>4.5</v>
+        <v>6.3</v>
       </c>
       <c r="D32" t="n">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -3651,32 +3651,32 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="B33" t="n">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
       <c r="C33" t="n">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="D33" t="n">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -3701,16 +3701,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="B34" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>5.8</v>
+        <v>5.5</v>
       </c>
       <c r="D34" t="n">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -3769,16 +3769,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>7.7</v>
+        <v>6.5</v>
       </c>
       <c r="B36" t="n">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
-        <v>6.7</v>
+        <v>5.5</v>
       </c>
       <c r="D36" t="n">
-        <v>2.2</v>
+        <v>1.8</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -3803,16 +3803,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="B37" t="n">
-        <v>3.2</v>
+        <v>2.2</v>
       </c>
       <c r="C37" t="n">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="D37" t="n">
-        <v>2.3</v>
+        <v>1.5</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -3821,32 +3821,32 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Iris-virginica</t>
+          <t>Iris-versicolor</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>7.2</v>
+        <v>6.7</v>
       </c>
       <c r="B38" t="n">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="D38" t="n">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -3871,16 +3871,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="B39" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C39" t="n">
-        <v>5.6</v>
+        <v>4.9</v>
       </c>
       <c r="D39" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -3905,16 +3905,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C40" t="n">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="D40" t="n">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3973,16 +3973,16 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" t="n">
         <v>6.1</v>
       </c>
-      <c r="B42" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="C42" t="n">
-        <v>5.6</v>
-      </c>
       <c r="D42" t="n">
-        <v>1.4</v>
+        <v>2.3</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Iris-versicolor</t>
+          <t>Iris-virginica</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -4007,16 +4007,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="B43" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="C43" t="n">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
       <c r="D43" t="n">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -4041,16 +4041,16 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="B44" t="n">
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="C44" t="n">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="D44" t="n">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -4075,13 +4075,13 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="C45" t="n">
-        <v>5.2</v>
+        <v>5.4</v>
       </c>
       <c r="D45" t="n">
         <v>2.3</v>
@@ -4109,16 +4109,16 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>6.3</v>
+        <v>5.9</v>
       </c>
       <c r="B46" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>5</v>
+        <v>5.1</v>
       </c>
       <c r="D46" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>

</xml_diff>